<commit_message>
Integration of optical switch.
</commit_message>
<xml_diff>
--- a/test0930-1.xlsx
+++ b/test0930-1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Date Time</t>
   </si>
@@ -155,6 +155,57 @@
   </si>
   <si>
     <t>Sat, 30 Sep 2017 16:39:31</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:40:57</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:42:35</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:43:16</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:51:40</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:52:14</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:52:40</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:53:06</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:53:34</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:54:01</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:54:26</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:54:52</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 16:55:17</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 17:08:57</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 17:09:40</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 17:10:23</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 17:11:03</t>
+  </si>
+  <si>
+    <t>Sat, 30 Sep 2017 17:11:45</t>
   </si>
 </sst>
 </file>
@@ -318,10 +369,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$148</c:f>
+              <c:f>Sheet1!$B$2:$B$267</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="147"/>
+                <c:ptCount val="266"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -383,6 +434,57 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -390,10 +492,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$2:$Z$148</c:f>
+              <c:f>Sheet1!$Z$2:$Z$267</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="147"/>
+                <c:ptCount val="266"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -455,6 +557,57 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -861,7 +1014,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z22"/>
+  <dimension ref="A1:Z39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3155,6 +3308,1791 @@
         <v>0</v>
       </c>
     </row>
+    <row r="23" spans="1:26">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23">
+        <f>VALUE(0.26229)</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="10">
+        <f>VALUE(1549.9896800000001)</f>
+        <v>0</v>
+      </c>
+      <c r="D23" s="10">
+        <f>VALUE(-11.698)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="11">
+        <f>VALUE(1551.06132)</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="11">
+        <f>VALUE(-18.374000000000002)</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="12">
+        <f>VALUE(1553.6967)</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="12">
+        <f>VALUE(-15.187999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="13">
+        <f>VALUE(1545.0266199999999)</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="13">
+        <f>VALUE(-10.777999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="K23" s="14">
+        <f>VALUE(1547.92716)</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="14">
+        <f>VALUE(-11.292)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="15">
+        <f>VALUE(1553.6244)</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="15">
+        <f>VALUE(-11.776)</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="16">
+        <f>VALUE(1548.58256)</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="16">
+        <f>VALUE(-21.031999999999996)</f>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="17">
+        <f>VALUE(300.046)</f>
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <f>VALUE(0.0012799999999515421)</f>
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <f>VALUE(0.0012200000001030276)</f>
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <f>VALUE(0.0012600000000020373)</f>
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <f>VALUE(0.0006400000002031447)</f>
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <f>VALUE(0.000839999999925567)</f>
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <f>VALUE(0.0010800000000017462)</f>
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <f>VALUE(0.00048000000015235855)</f>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="17">
+        <f>VALUE(0.12700000000000955)</f>
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <f>VALUE(0.9714285714770605)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24">
+        <f>VALUE(0.28959)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="10">
+        <f>VALUE(1549.9927599999999)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="10">
+        <f>VALUE(-11.61)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="11">
+        <f>VALUE(1551.06306)</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="11">
+        <f>VALUE(-18.386)</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="12">
+        <f>VALUE(1553.70056)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="12">
+        <f>VALUE(-15.228)</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="13">
+        <f>VALUE(1545.02882)</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="13">
+        <f>VALUE(-10.798)</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="14">
+        <f>VALUE(1547.92864)</f>
+        <v>0</v>
+      </c>
+      <c r="L24" s="14">
+        <f>VALUE(-11.288)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="15">
+        <f>VALUE(1553.62702)</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="15">
+        <f>VALUE(-11.738)</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="16">
+        <f>VALUE(1548.58264)</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="16">
+        <f>VALUE(-20.96)</f>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="17">
+        <f>VALUE(300.09999999999997)</f>
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <f>VALUE(0.004360000000133368)</f>
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <f>VALUE(0.0029600000000300497)</f>
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <f>VALUE(0.005120000000033542)</f>
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <f>VALUE(0.002840000000105647)</f>
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <f>VALUE(0.0023200000000542786)</f>
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <f>VALUE(0.0036999999999807187)</f>
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <f>VALUE(0.0005600000001777516)</f>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="17">
+        <f>VALUE(0.18099999999998317)</f>
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <f>VALUE(3.122857142930765)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <f>VALUE(0.30098)</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="10">
+        <f>VALUE(1549.99404)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="10">
+        <f>VALUE(-11.618)</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="11">
+        <f>VALUE(1551.06446)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="11">
+        <f>VALUE(-18.354)</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="12">
+        <f>VALUE(1553.7029)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="12">
+        <f>VALUE(-15.238)</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="13">
+        <f>VALUE(1545.02982)</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="13">
+        <f>VALUE(-10.815999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="14">
+        <f>VALUE(1547.93134)</f>
+        <v>0</v>
+      </c>
+      <c r="L25" s="14">
+        <f>VALUE(-11.324000000000002)</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="15">
+        <f>VALUE(1553.6300199999998)</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="15">
+        <f>VALUE(-11.76)</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="16">
+        <f>VALUE(1548.58318)</f>
+        <v>0</v>
+      </c>
+      <c r="P25" s="16">
+        <f>VALUE(-21.002)</f>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="17">
+        <f>VALUE(300.1805)</f>
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <f>VALUE(0.00564000000008491)</f>
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <f>VALUE(0.004360000000133368)</f>
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <f>VALUE(0.007460000000037326)</f>
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <f>VALUE(0.003840000000082)</f>
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <f>VALUE(0.005020000000058644)</f>
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <f>VALUE(0.006700000000137152)</f>
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <f>VALUE(0.0011000000001786248)</f>
+        <v>0</v>
+      </c>
+      <c r="Y25" s="17">
+        <f>VALUE(0.2615000000000123)</f>
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <f>VALUE(4.874285714387432)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <f>VALUE(0.44098)</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="10">
+        <f>VALUE(1550.0431800000001)</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="10">
+        <f>VALUE(-11.66)</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="11">
+        <f>VALUE(1551.0884)</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="11">
+        <f>VALUE(-18.375999999999998)</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
+        <f>VALUE(1553.76396)</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <f>VALUE(-15.216)</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="13">
+        <f>VALUE(1545.05136)</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="13">
+        <f>VALUE(-10.794)</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="14">
+        <f>VALUE(1547.9505800000002)</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="14">
+        <f>VALUE(-11.306)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="15">
+        <f>VALUE(1553.66524)</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="15">
+        <f>VALUE(-11.687999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="16">
+        <f>VALUE(1548.58346)</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="16">
+        <f>VALUE(-20.996)</f>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="17">
+        <f>VALUE(301.97999999999996)</f>
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <f>VALUE(0.05477999999993699)</f>
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <f>VALUE(0.028300000000172076)</f>
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <f>VALUE(0.068520000000035)</f>
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <f>VALUE(0.025380000000041036)</f>
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <f>VALUE(0.024259999999912907)</f>
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <f>VALUE(0.04192000000011831)</f>
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <f>VALUE(0.0013800000001538137)</f>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="17">
+        <f>VALUE(2.0609999999999786)</f>
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <f>VALUE(34.93428571433859)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <f>VALUE(0.45045)</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="10">
+        <f>VALUE(1550.14032)</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="10">
+        <f>VALUE(-11.665999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="11">
+        <f>VALUE(1551.12422)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="11">
+        <f>VALUE(-18.372)</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="12">
+        <f>VALUE(1553.8814)</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="12">
+        <f>VALUE(-15.216)</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="13">
+        <f>VALUE(1545.08284)</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="13">
+        <f>VALUE(-10.748)</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="14">
+        <f>VALUE(1547.97356)</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="14">
+        <f>VALUE(-11.32)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="15">
+        <f>VALUE(1553.7371)</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="15">
+        <f>VALUE(-11.752)</f>
+        <v>0</v>
+      </c>
+      <c r="O27" s="16">
+        <f>VALUE(1548.58302)</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="16">
+        <f>VALUE(-20.958000000000002)</f>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="17">
+        <f>VALUE(303.0625)</f>
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <f>VALUE(0.15192000000001826)</f>
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <f>VALUE(0.06412000000000262)</f>
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <f>VALUE(0.18596000000002277)</f>
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <f>VALUE(0.05686000000014246)</f>
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <f>VALUE(0.04723999999987427)</f>
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <f>VALUE(0.11378000000013344)</f>
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <f>VALUE(0.0009400000001278386)</f>
+        <v>0</v>
+      </c>
+      <c r="Y27" s="17">
+        <f>VALUE(3.1435000000000173)</f>
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <f>VALUE(88.68857142861738)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28">
+        <f>VALUE(0.45779)</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="10">
+        <f>VALUE(1550.2177800000002)</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="10">
+        <f>VALUE(-11.692)</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="11">
+        <f>VALUE(1551.16238)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="11">
+        <f>VALUE(-18.32)</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="12">
+        <f>VALUE(1553.96856)</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="12">
+        <f>VALUE(-15.204)</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="13">
+        <f>VALUE(1545.1159)</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="13">
+        <f>VALUE(-10.804)</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="14">
+        <f>VALUE(1548.00092)</f>
+        <v>0</v>
+      </c>
+      <c r="L28" s="14">
+        <f>VALUE(-11.265999999999998)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="15">
+        <f>VALUE(1553.79464)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="15">
+        <f>VALUE(-11.777999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="O28" s="16">
+        <f>VALUE(1548.58364)</f>
+        <v>0</v>
+      </c>
+      <c r="P28" s="16">
+        <f>VALUE(-20.912)</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="17">
+        <f>VALUE(304.46549999999996)</f>
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <f>VALUE(0.22937999999999192)</f>
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <f>VALUE(0.10228000000006432)</f>
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <f>VALUE(0.27312000000006265)</f>
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <f>VALUE(0.08992000000012013)</f>
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <f>VALUE(0.07459999999991851)</f>
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <f>VALUE(0.17132000000015069)</f>
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <f>VALUE(0.0015600000001541048)</f>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="17">
+        <f>VALUE(4.5464999999999804)</f>
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <f>VALUE(134.5971428572089)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29">
+        <f>VALUE(0.46488)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="10">
+        <f>VALUE(1550.2997599999999)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="10">
+        <f>VALUE(-11.687999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="11">
+        <f>VALUE(1551.2068199999999)</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="11">
+        <f>VALUE(-18.346)</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="12">
+        <f>VALUE(1554.05628)</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="12">
+        <f>VALUE(-15.196)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="13">
+        <f>VALUE(1545.15376)</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="13">
+        <f>VALUE(-10.764000000000001)</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="14">
+        <f>VALUE(1548.03456)</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="14">
+        <f>VALUE(-11.276)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="15">
+        <f>VALUE(1553.85512)</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="15">
+        <f>VALUE(-11.69)</f>
+        <v>0</v>
+      </c>
+      <c r="O29" s="16">
+        <f>VALUE(1548.58332)</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="16">
+        <f>VALUE(-20.97)</f>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="17">
+        <f>VALUE(306.2795)</f>
+        <v>0</v>
+      </c>
+      <c r="R29">
+        <f>VALUE(0.31136000000014974)</f>
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <f>VALUE(0.1467200000001867)</f>
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <f>VALUE(0.3608400000000529)</f>
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <f>VALUE(0.12778000000002976)</f>
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <f>VALUE(0.10824000000002343)</f>
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <f>VALUE(0.2318000000000211)</f>
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <f>VALUE(0.0012400000000525324)</f>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="17">
+        <f>VALUE(6.360500000000002)</f>
+        <v>0</v>
+      </c>
+      <c r="Z29">
+        <f>VALUE(183.9971428572166)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30">
+        <f>VALUE(0.47258)</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="10">
+        <f>VALUE(1550.38348)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="10">
+        <f>VALUE(-11.725999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="11">
+        <f>VALUE(1551.2599599999999)</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="11">
+        <f>VALUE(-18.35)</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="12">
+        <f>VALUE(1554.14546)</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="12">
+        <f>VALUE(-15.218)</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="13">
+        <f>VALUE(1545.19776)</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="13">
+        <f>VALUE(-10.782)</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="14">
+        <f>VALUE(1548.0762)</f>
+        <v>0</v>
+      </c>
+      <c r="L30" s="14">
+        <f>VALUE(-11.31)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="15">
+        <f>VALUE(1553.91758)</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="15">
+        <f>VALUE(-11.752)</f>
+        <v>0</v>
+      </c>
+      <c r="O30" s="16">
+        <f>VALUE(1548.5836800000002)</f>
+        <v>0</v>
+      </c>
+      <c r="P30" s="16">
+        <f>VALUE(-20.98)</f>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="17">
+        <f>VALUE(308.5195)</f>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f>VALUE(0.3950800000000072)</f>
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <f>VALUE(0.19986000000017157)</f>
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <f>VALUE(0.450019999999995)</f>
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <f>VALUE(0.17178000000012617)</f>
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <f>VALUE(0.14987999999993917)</f>
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <f>VALUE(0.2942600000001221)</f>
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <f>VALUE(0.0016000000000531145)</f>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="17">
+        <f>VALUE(8.600500000000011)</f>
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <f>VALUE(237.49714285720205)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31">
+        <f>VALUE(0.48015)</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="10">
+        <f>VALUE(1550.4696800000002)</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="10">
+        <f>VALUE(-11.628)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="11">
+        <f>VALUE(1551.31554)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="11">
+        <f>VALUE(-18.364)</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="12">
+        <f>VALUE(1554.23378)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="12">
+        <f>VALUE(-15.155999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="13">
+        <f>VALUE(1545.24736)</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="13">
+        <f>VALUE(-10.758)</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="14">
+        <f>VALUE(1548.12556)</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="14">
+        <f>VALUE(-11.298)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="15">
+        <f>VALUE(1553.9839)</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="15">
+        <f>VALUE(-11.65)</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="16">
+        <f>VALUE(1548.58438)</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="16">
+        <f>VALUE(-20.944000000000003)</f>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="17">
+        <f>VALUE(311.229)</f>
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f>VALUE(0.48127999999996973)</f>
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <f>VALUE(0.2554400000001351)</f>
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <f>VALUE(0.538340000000062)</f>
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <f>VALUE(0.2213800000001811)</f>
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <f>VALUE(0.19923999999991793)</f>
+        <v>0</v>
+      </c>
+      <c r="W31">
+        <f>VALUE(0.3605800000000272)</f>
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <f>VALUE(0.002300000000104774)</f>
+        <v>0</v>
+      </c>
+      <c r="Y31" s="17">
+        <f>VALUE(11.310000000000002)</f>
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <f>VALUE(294.0800000000568)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26">
+      <c r="A32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <f>VALUE(0.48724)</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="10">
+        <f>VALUE(1550.5479)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="10">
+        <f>VALUE(-11.665999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="11">
+        <f>VALUE(1551.37208)</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="11">
+        <f>VALUE(-18.27)</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="12">
+        <f>VALUE(1554.31512)</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="12">
+        <f>VALUE(-15.155999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="13">
+        <f>VALUE(1545.29824)</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="13">
+        <f>VALUE(-10.802)</f>
+        <v>0</v>
+      </c>
+      <c r="K32" s="14">
+        <f>VALUE(1548.17652)</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="14">
+        <f>VALUE(-11.332)</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="15">
+        <f>VALUE(1554.04778)</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="15">
+        <f>VALUE(-11.718)</f>
+        <v>0</v>
+      </c>
+      <c r="O32" s="16">
+        <f>VALUE(1548.58408)</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="16">
+        <f>VALUE(-20.962)</f>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="17">
+        <f>VALUE(314.215)</f>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f>VALUE(0.5595000000000709)</f>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f>VALUE(0.311980000000176)</f>
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <f>VALUE(0.6196800000000167)</f>
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f>VALUE(0.2722600000001876)</f>
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <f>VALUE(0.2501999999999498)</f>
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <f>VALUE(0.424460000000181)</f>
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <f>VALUE(0.00200000000018008)</f>
+        <v>0</v>
+      </c>
+      <c r="Y32" s="17">
+        <f>VALUE(14.295999999999992)</f>
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <f>VALUE(348.582857142966)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33">
+        <f>VALUE(0.49422)</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="10">
+        <f>VALUE(1550.6268599999999)</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="10">
+        <f>VALUE(-11.692)</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="11">
+        <f>VALUE(1551.4312)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="11">
+        <f>VALUE(-18.328)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="12">
+        <f>VALUE(1554.39616)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="12">
+        <f>VALUE(-15.218)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="13">
+        <f>VALUE(1545.3533400000001)</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="13">
+        <f>VALUE(-10.79)</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="14">
+        <f>VALUE(1548.2313199999999)</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="14">
+        <f>VALUE(-11.218)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="15">
+        <f>VALUE(1554.11218)</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="15">
+        <f>VALUE(-11.745999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="O33" s="16">
+        <f>VALUE(1548.5838)</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="16">
+        <f>VALUE(-20.932)</f>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="17">
+        <f>VALUE(317.409)</f>
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <f>VALUE(0.6384600000001228)</f>
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <f>VALUE(0.3711000000000695)</f>
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <f>VALUE(0.7007200000000466)</f>
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <f>VALUE(0.32735999999999876)</f>
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <f>VALUE(0.30500000000006366)</f>
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <f>VALUE(0.48886000000015883)</f>
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <f>VALUE(0.001720000000204891)</f>
+        <v>0</v>
+      </c>
+      <c r="Y33" s="17">
+        <f>VALUE(17.49000000000001)</f>
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <f>VALUE(404.7457142858093)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34">
+        <f>VALUE(0.50115)</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="10">
+        <f>VALUE(1550.70076)</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="10">
+        <f>VALUE(-11.684000000000001)</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="11">
+        <f>VALUE(1551.48896)</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="11">
+        <f>VALUE(-18.264)</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="12">
+        <f>VALUE(1554.4715199999998)</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="12">
+        <f>VALUE(-15.186)</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="13">
+        <f>VALUE(1545.40918)</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="13">
+        <f>VALUE(-10.815999999999999)</f>
+        <v>0</v>
+      </c>
+      <c r="K34" s="14">
+        <f>VALUE(1548.28726)</f>
+        <v>0</v>
+      </c>
+      <c r="L34" s="14">
+        <f>VALUE(-11.26)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="15">
+        <f>VALUE(1554.1749)</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="15">
+        <f>VALUE(-11.68)</f>
+        <v>0</v>
+      </c>
+      <c r="O34" s="16">
+        <f>VALUE(1548.5842599999999)</f>
+        <v>0</v>
+      </c>
+      <c r="P34" s="16">
+        <f>VALUE(-20.908)</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="17">
+        <f>VALUE(320.85749999999996)</f>
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <f>VALUE(0.7123599999999897)</f>
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <f>VALUE(0.42885999999998603)</f>
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <f>VALUE(0.7760800000000927)</f>
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <f>VALUE(0.38320000000021537)</f>
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <f>VALUE(0.3609400000000278)</f>
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <f>VALUE(0.5515800000000581)</f>
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <f>VALUE(0.002180000000180371)</f>
+        <v>0</v>
+      </c>
+      <c r="Y34" s="17">
+        <f>VALUE(20.938499999999976)</f>
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <f>VALUE(459.3142857143643)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35">
+        <f>VALUE(0.72896)</f>
+        <v>0</v>
+      </c>
+      <c r="C35" s="10">
+        <f>VALUE(1552.62978)</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="10">
+        <f>VALUE(-11.6)</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="11">
+        <f>VALUE(1553.41222)</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="11">
+        <f>VALUE(-18.227999999999998)</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="12">
+        <f>VALUE(1556.41914)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="12">
+        <f>VALUE(-15.15)</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="13">
+        <f>VALUE(1547.30788)</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="13">
+        <f>VALUE(-10.774000000000001)</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="14">
+        <f>VALUE(1550.21046)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="14">
+        <f>VALUE(-11.328)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="15">
+        <f>VALUE(1556.08546)</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="15">
+        <f>VALUE(-11.708)</f>
+        <v>0</v>
+      </c>
+      <c r="O35" s="16">
+        <f>VALUE(1548.58448)</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="16">
+        <f>VALUE(-20.9)</f>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="17">
+        <f>VALUE(474.7725)</f>
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <f>VALUE(2.6413800000000265)</f>
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <f>VALUE(2.3521200000000135)</f>
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <f>VALUE(2.723700000000008)</f>
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <f>VALUE(2.281900000000178)</f>
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <f>VALUE(2.2841399999999794)</f>
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <f>VALUE(2.4621400000000904)</f>
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <f>VALUE(0.0024000000000796717)</f>
+        <v>0</v>
+      </c>
+      <c r="Y35" s="17">
+        <f>VALUE(174.8535)</f>
+        <v>0</v>
+      </c>
+      <c r="Z35">
+        <f>VALUE(2106.825714285768)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36">
+        <f>VALUE(0.74099)</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="10">
+        <f>VALUE(1552.70554)</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="10">
+        <f>VALUE(-11.61)</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="11">
+        <f>VALUE(1553.49578)</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="11">
+        <f>VALUE(-18.24)</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="12">
+        <f>VALUE(1556.4976199999999)</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <f>VALUE(-15.114)</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="13">
+        <f>VALUE(1547.39052)</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="13">
+        <f>VALUE(-10.78)</f>
+        <v>0</v>
+      </c>
+      <c r="K36" s="14">
+        <f>VALUE(1550.29566)</f>
+        <v>0</v>
+      </c>
+      <c r="L36" s="14">
+        <f>VALUE(-11.294)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="15">
+        <f>VALUE(1556.16872)</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="15">
+        <f>VALUE(-11.702)</f>
+        <v>0</v>
+      </c>
+      <c r="O36" s="16">
+        <f>VALUE(1548.5845)</f>
+        <v>0</v>
+      </c>
+      <c r="P36" s="16">
+        <f>VALUE(-20.901999999999997)</f>
+        <v>0</v>
+      </c>
+      <c r="Q36" s="17">
+        <f>VALUE(481.6785)</f>
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <f>VALUE(2.717139999999972)</f>
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <f>VALUE(2.4356800000000476)</f>
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <f>VALUE(2.802180000000135)</f>
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <f>VALUE(2.3645400000000336)</f>
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <f>VALUE(2.3693399999999656)</f>
+        <v>0</v>
+      </c>
+      <c r="W36">
+        <f>VALUE(2.5453999999999724)</f>
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <f>VALUE(0.0024200000000291766)</f>
+        <v>0</v>
+      </c>
+      <c r="Y36" s="17">
+        <f>VALUE(181.7595)</f>
+        <v>0</v>
+      </c>
+      <c r="Z36">
+        <f>VALUE(2176.6714285714506)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37">
+        <f>VALUE(0.753)</f>
+        <v>0</v>
+      </c>
+      <c r="C37" s="10">
+        <f>VALUE(1552.77812)</f>
+        <v>0</v>
+      </c>
+      <c r="D37" s="10">
+        <f>VALUE(-11.602)</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="11">
+        <f>VALUE(1553.58048)</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="11">
+        <f>VALUE(-18.224)</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="12">
+        <f>VALUE(1556.58262)</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="12">
+        <f>VALUE(-15.112)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="13">
+        <f>VALUE(1547.4769800000001)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="13">
+        <f>VALUE(-10.818)</f>
+        <v>0</v>
+      </c>
+      <c r="K37" s="14">
+        <f>VALUE(1550.38122)</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="14">
+        <f>VALUE(-11.296)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="15">
+        <f>VALUE(1556.2511)</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="15">
+        <f>VALUE(-11.718)</f>
+        <v>0</v>
+      </c>
+      <c r="O37" s="16">
+        <f>VALUE(1548.58486)</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="16">
+        <f>VALUE(-20.886)</f>
+        <v>0</v>
+      </c>
+      <c r="Q37" s="17">
+        <f>VALUE(488.672)</f>
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <f>VALUE(2.7897199999999884)</f>
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <f>VALUE(2.5203800000001593)</f>
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <f>VALUE(2.887179999999944)</f>
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <f>VALUE(2.451000000000022)</f>
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <f>VALUE(2.4548999999999523)</f>
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <f>VALUE(2.6277800000000298)</f>
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <f>VALUE(0.0027800000000297587)</f>
+        <v>0</v>
+      </c>
+      <c r="Y37" s="17">
+        <f>VALUE(188.75300000000004)</f>
+        <v>0</v>
+      </c>
+      <c r="Z37">
+        <f>VALUE(2247.6771428571606)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26">
+      <c r="A38" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38">
+        <f>VALUE(0.76411)</f>
+        <v>0</v>
+      </c>
+      <c r="C38" s="10">
+        <f>VALUE(1552.84626)</f>
+        <v>0</v>
+      </c>
+      <c r="D38" s="10">
+        <f>VALUE(-11.632)</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="11">
+        <f>VALUE(1553.66006)</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="11">
+        <f>VALUE(-18.248)</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="12">
+        <f>VALUE(1556.6570800000002)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="12">
+        <f>VALUE(-15.122)</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="13">
+        <f>VALUE(1547.5583)</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="13">
+        <f>VALUE(-10.822000000000001)</f>
+        <v>0</v>
+      </c>
+      <c r="K38" s="14">
+        <f>VALUE(1550.46208)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="14">
+        <f>VALUE(-11.314)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="15">
+        <f>VALUE(1556.32888)</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="15">
+        <f>VALUE(-11.672)</f>
+        <v>0</v>
+      </c>
+      <c r="O38" s="16">
+        <f>VALUE(1548.58484)</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="16">
+        <f>VALUE(-20.9)</f>
+        <v>0</v>
+      </c>
+      <c r="Q38" s="17">
+        <f>VALUE(495.1825)</f>
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <f>VALUE(2.8578600000000733)</f>
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <f>VALUE(2.59996000000001)</f>
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <f>VALUE(2.9616399999999885)</f>
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <f>VALUE(2.532320000000027)</f>
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <f>VALUE(2.535759999999982)</f>
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <f>VALUE(2.705560000000105)</f>
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <f>VALUE(0.002760000000080254)</f>
+        <v>0</v>
+      </c>
+      <c r="Y38" s="17">
+        <f>VALUE(195.26350000000002)</f>
+        <v>0</v>
+      </c>
+      <c r="Z38">
+        <f>VALUE(2313.6942857143235)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39">
+        <f>VALUE(0.77571)</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="10">
+        <f>VALUE(1552.9103400000001)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="10">
+        <f>VALUE(-11.606)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="11">
+        <f>VALUE(1553.7356)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="11">
+        <f>VALUE(-18.25)</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="12">
+        <f>VALUE(1556.72044)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="12">
+        <f>VALUE(-15.078)</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="13">
+        <f>VALUE(1547.63508)</f>
+        <v>0</v>
+      </c>
+      <c r="J39" s="13">
+        <f>VALUE(-10.818)</f>
+        <v>0</v>
+      </c>
+      <c r="K39" s="14">
+        <f>VALUE(1550.53988)</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="14">
+        <f>VALUE(-11.244000000000002)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="15">
+        <f>VALUE(1556.4019)</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="15">
+        <f>VALUE(-11.692)</f>
+        <v>0</v>
+      </c>
+      <c r="O39" s="16">
+        <f>VALUE(1548.5851)</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="16">
+        <f>VALUE(-20.87)</f>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="17">
+        <f>VALUE(501.447)</f>
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <f>VALUE(2.9219399999999496)</f>
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <f>VALUE(2.6755000000000564)</f>
+        <v>0</v>
+      </c>
+      <c r="T39">
+        <f>VALUE(3.025000000000091)</f>
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <f>VALUE(2.609100000000126)</f>
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <f>VALUE(2.6135600000000068)</f>
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <f>VALUE(2.7785800000001473)</f>
+        <v>0</v>
+      </c>
+      <c r="X39">
+        <f>VALUE(0.003020000000105938)</f>
+        <v>0</v>
+      </c>
+      <c r="Y39" s="17">
+        <f>VALUE(201.52800000000002)</f>
+        <v>0</v>
+      </c>
+      <c r="Z39">
+        <f>VALUE(2375.242857142926)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>